<commit_message>
Updated DEU model - 2025-08-31 14:42
</commit_message>
<xml_diff>
--- a/VerveStacks_DEU/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_DEU/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_DEU\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{55179210-A823-4FF0-A5CB-686AB6AB9B8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{15284001-B827-4E3F-9E56-A73472D5019C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2246" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2246" uniqueCount="543">
   <si>
     <t>~FI_Process</t>
   </si>
@@ -1745,6 +1745,9 @@
   </si>
   <si>
     <t>Wind offshore</t>
+  </si>
+  <si>
+    <t>unknown</t>
   </si>
   <si>
     <t>Wind onshore</t>
@@ -2797,7 +2800,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C183C4E3-6B03-DCC9-AC6B-9D290B00ED33}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3C82396-8B08-8A24-3987-AFBAD8E83DDB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2852,7 +2855,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{469B5564-95C2-4D41-4EC4-2235BFF2310A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05357143-C91B-FBCE-5FD4-A6B42DEFD392}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2907,7 +2910,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BEEB80E4-0804-CA22-51F1-C860A495FAE7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B5364EB-C085-6464-1DE4-ACE3477E6104}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2962,7 +2965,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9B90310-1A00-9D3D-CE01-7CD44291780F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B01B09E-A888-834A-38D3-91F3E7813CD2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6892,7 +6895,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3886466-D9F7-43DF-8C5F-0FBEF770D2C1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCEC3FE8-78C7-4F13-B4D9-AD3979207FE1}">
   <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7969,7 +7972,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7A6BDB2-DA76-4D5A-8E7A-6A5F2E53F775}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{105A63B8-1C05-498C-BFE3-B670ACDAE17E}">
   <dimension ref="A1:P147"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13966,7 +13969,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1852C978-D09E-44BC-B6AA-B6761ED9B5BA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEF17CCD-954E-47F2-90E3-1E1D1A00A55E}">
   <dimension ref="A1:Q66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -14084,10 +14087,10 @@
         <v>21</v>
       </c>
       <c r="P4" s="156" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="Q4" s="156" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -14126,10 +14129,10 @@
         <v>21</v>
       </c>
       <c r="P5" s="157" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="Q5" s="157" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -14168,10 +14171,10 @@
         <v>21</v>
       </c>
       <c r="P6" s="156" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="Q6" s="156" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -14210,10 +14213,10 @@
         <v>21</v>
       </c>
       <c r="P7" s="157" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="Q7" s="157" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -14252,10 +14255,10 @@
         <v>21</v>
       </c>
       <c r="P8" s="156" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="Q8" s="156" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -14294,10 +14297,10 @@
         <v>21</v>
       </c>
       <c r="P9" s="157" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="Q9" s="157" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -14336,10 +14339,10 @@
         <v>21</v>
       </c>
       <c r="P10" s="156" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="Q10" s="156" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -14378,10 +14381,10 @@
         <v>21</v>
       </c>
       <c r="P11" s="157" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="Q11" s="157" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -14420,10 +14423,10 @@
         <v>21</v>
       </c>
       <c r="P12" s="156" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="Q12" s="156" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -14462,10 +14465,10 @@
         <v>21</v>
       </c>
       <c r="P13" s="157" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="Q13" s="157" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -14504,10 +14507,10 @@
         <v>21</v>
       </c>
       <c r="P14" s="156" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="Q14" s="156" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -14546,10 +14549,10 @@
         <v>21</v>
       </c>
       <c r="P15" s="157" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="Q15" s="157" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -14588,10 +14591,10 @@
         <v>21</v>
       </c>
       <c r="P16" s="156" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="Q16" s="156" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="17" spans="2:17">
@@ -14630,10 +14633,10 @@
         <v>21</v>
       </c>
       <c r="P17" s="157" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="Q17" s="157" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="18" spans="2:17">
@@ -14672,10 +14675,10 @@
         <v>21</v>
       </c>
       <c r="P18" s="156" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="Q18" s="156" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="19" spans="2:17">
@@ -14714,10 +14717,10 @@
         <v>21</v>
       </c>
       <c r="P19" s="157" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="Q19" s="157" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="20" spans="2:17">
@@ -14746,7 +14749,7 @@
         <v>172</v>
       </c>
       <c r="L20" s="156" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="M20" s="156"/>
       <c r="N20" s="156" t="s">
@@ -14756,10 +14759,10 @@
         <v>21</v>
       </c>
       <c r="P20" s="156" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="Q20" s="156" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="21" spans="2:17">
@@ -15595,7 +15598,7 @@
         <v>538</v>
       </c>
       <c r="C57" s="157" t="s">
-        <v>28</v>
+        <v>539</v>
       </c>
       <c r="D57" s="157" t="s">
         <v>19</v>
@@ -15618,7 +15621,7 @@
         <v>538</v>
       </c>
       <c r="C58" s="156" t="s">
-        <v>28</v>
+        <v>539</v>
       </c>
       <c r="D58" s="156" t="s">
         <v>19</v>
@@ -15641,7 +15644,7 @@
         <v>538</v>
       </c>
       <c r="C59" s="157" t="s">
-        <v>28</v>
+        <v>539</v>
       </c>
       <c r="D59" s="157" t="s">
         <v>19</v>
@@ -15664,7 +15667,7 @@
         <v>538</v>
       </c>
       <c r="C60" s="156" t="s">
-        <v>28</v>
+        <v>539</v>
       </c>
       <c r="D60" s="156" t="s">
         <v>19</v>
@@ -15687,7 +15690,7 @@
         <v>538</v>
       </c>
       <c r="C61" s="157" t="s">
-        <v>28</v>
+        <v>539</v>
       </c>
       <c r="D61" s="157" t="s">
         <v>19</v>
@@ -15707,10 +15710,10 @@
     </row>
     <row r="62" spans="2:8">
       <c r="B62" s="156" t="s">
+        <v>540</v>
+      </c>
+      <c r="C62" s="156" t="s">
         <v>539</v>
-      </c>
-      <c r="C62" s="156" t="s">
-        <v>28</v>
       </c>
       <c r="D62" s="156" t="s">
         <v>19</v>
@@ -15730,10 +15733,10 @@
     </row>
     <row r="63" spans="2:8">
       <c r="B63" s="157" t="s">
+        <v>540</v>
+      </c>
+      <c r="C63" s="157" t="s">
         <v>539</v>
-      </c>
-      <c r="C63" s="157" t="s">
-        <v>28</v>
       </c>
       <c r="D63" s="157" t="s">
         <v>19</v>
@@ -15753,10 +15756,10 @@
     </row>
     <row r="64" spans="2:8">
       <c r="B64" s="156" t="s">
+        <v>540</v>
+      </c>
+      <c r="C64" s="156" t="s">
         <v>539</v>
-      </c>
-      <c r="C64" s="156" t="s">
-        <v>28</v>
       </c>
       <c r="D64" s="156" t="s">
         <v>19</v>
@@ -15776,10 +15779,10 @@
     </row>
     <row r="65" spans="2:8">
       <c r="B65" s="157" t="s">
+        <v>540</v>
+      </c>
+      <c r="C65" s="157" t="s">
         <v>539</v>
-      </c>
-      <c r="C65" s="157" t="s">
-        <v>28</v>
       </c>
       <c r="D65" s="157" t="s">
         <v>19</v>
@@ -15799,10 +15802,10 @@
     </row>
     <row r="66" spans="2:8">
       <c r="B66" s="156" t="s">
+        <v>540</v>
+      </c>
+      <c r="C66" s="156" t="s">
         <v>539</v>
-      </c>
-      <c r="C66" s="156" t="s">
-        <v>28</v>
       </c>
       <c r="D66" s="156" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Updated DEU model - 2025-08-31 17:04
</commit_message>
<xml_diff>
--- a/VerveStacks_DEU/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_DEU/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_DEU\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{15284001-B827-4E3F-9E56-A73472D5019C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C757E023-CD8A-493C-A95B-136D37ABFDA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2800,7 +2800,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3C82396-8B08-8A24-3987-AFBAD8E83DDB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FBB6F41-C5A0-3465-8089-61AC53F5CA8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2855,7 +2855,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05357143-C91B-FBCE-5FD4-A6B42DEFD392}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C91DD294-1AC8-23BD-E314-E527FCD4D2C7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2910,7 +2910,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B5364EB-C085-6464-1DE4-ACE3477E6104}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73411106-AD71-3FF4-26B2-EF26518D6356}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2965,7 +2965,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B01B09E-A888-834A-38D3-91F3E7813CD2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44B9F7E3-58D7-F7E6-ED1A-DF37DFA1B5E8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6895,7 +6895,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCEC3FE8-78C7-4F13-B4D9-AD3979207FE1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31BDA319-AB55-4511-8966-E89D9648B514}">
   <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7972,7 +7972,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{105A63B8-1C05-498C-BFE3-B670ACDAE17E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C84FC64-FA23-4FAC-B368-CCB4DD3A4433}">
   <dimension ref="A1:P147"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13969,7 +13969,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEF17CCD-954E-47F2-90E3-1E1D1A00A55E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9D93A9B-F785-43FF-826A-718D3FA73717}">
   <dimension ref="A1:Q66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated DEU model - 2025-08-31 17:15
</commit_message>
<xml_diff>
--- a/VerveStacks_DEU/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_DEU/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_DEU\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C757E023-CD8A-493C-A95B-136D37ABFDA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{538F5984-CAE0-4484-841E-E6FFF7C2F564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2800,7 +2800,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FBB6F41-C5A0-3465-8089-61AC53F5CA8A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B103C88-1CB9-292F-246D-297CA8118BF8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2855,7 +2855,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C91DD294-1AC8-23BD-E314-E527FCD4D2C7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97EFFCA5-4B02-ACF4-B862-C746345F32B3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2910,7 +2910,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73411106-AD71-3FF4-26B2-EF26518D6356}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12B424EA-B8CD-8A77-A181-8B6FB1A10D5F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2965,7 +2965,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44B9F7E3-58D7-F7E6-ED1A-DF37DFA1B5E8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA79CD9B-17E1-BEE2-A316-2AAE6370FB8F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6895,7 +6895,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31BDA319-AB55-4511-8966-E89D9648B514}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0B4A611-D73C-41EA-B2AB-C0CF3F1C6711}">
   <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7972,7 +7972,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C84FC64-FA23-4FAC-B368-CCB4DD3A4433}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF3FDB3C-3379-42BA-8052-1F6201163294}">
   <dimension ref="A1:P147"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13969,7 +13969,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9D93A9B-F785-43FF-826A-718D3FA73717}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02D1E3E1-4F4D-4CCB-BDDC-DC9B9ECE648A}">
   <dimension ref="A1:Q66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated DEU model - 2025-08-31 19:06
</commit_message>
<xml_diff>
--- a/VerveStacks_DEU/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_DEU/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_DEU\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C050752-66BE-414E-975D-69E1F69292DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7FB87C35-88B3-4BAD-84FA-21BE7444021E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2246" uniqueCount="543">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2584" uniqueCount="616">
   <si>
     <t>~FI_Process</t>
   </si>
@@ -1682,6 +1682,225 @@
   </si>
   <si>
     <t>elc_won-DEU</t>
+  </si>
+  <si>
+    <t>e_wof-DEU_59_c3</t>
+  </si>
+  <si>
+    <t>offshore wind resource -- CF class wof-DEU_59 -- cost class 3</t>
+  </si>
+  <si>
+    <t>e_wof-DEU_59_c5</t>
+  </si>
+  <si>
+    <t>offshore wind resource -- CF class wof-DEU_59 -- cost class 5</t>
+  </si>
+  <si>
+    <t>e_wof-DEU_59_c2</t>
+  </si>
+  <si>
+    <t>offshore wind resource -- CF class wof-DEU_59 -- cost class 2</t>
+  </si>
+  <si>
+    <t>e_wof-DEU_59_c4</t>
+  </si>
+  <si>
+    <t>offshore wind resource -- CF class wof-DEU_59 -- cost class 4</t>
+  </si>
+  <si>
+    <t>e_wof-DEU_59_c1</t>
+  </si>
+  <si>
+    <t>offshore wind resource -- CF class wof-DEU_59 -- cost class 1</t>
+  </si>
+  <si>
+    <t>e_wof-DEU_58_c3</t>
+  </si>
+  <si>
+    <t>offshore wind resource -- CF class wof-DEU_58 -- cost class 3</t>
+  </si>
+  <si>
+    <t>e_wof-DEU_58_c2</t>
+  </si>
+  <si>
+    <t>offshore wind resource -- CF class wof-DEU_58 -- cost class 2</t>
+  </si>
+  <si>
+    <t>e_wof-DEU_58_c1</t>
+  </si>
+  <si>
+    <t>offshore wind resource -- CF class wof-DEU_58 -- cost class 1</t>
+  </si>
+  <si>
+    <t>e_wof-DEU_57_c2</t>
+  </si>
+  <si>
+    <t>offshore wind resource -- CF class wof-DEU_57 -- cost class 2</t>
+  </si>
+  <si>
+    <t>e_wof-DEU_57_c1</t>
+  </si>
+  <si>
+    <t>offshore wind resource -- CF class wof-DEU_57 -- cost class 1</t>
+  </si>
+  <si>
+    <t>e_wof-DEU_56_c1</t>
+  </si>
+  <si>
+    <t>offshore wind resource -- CF class wof-DEU_56 -- cost class 1</t>
+  </si>
+  <si>
+    <t>e_wof-DEU_55_c1</t>
+  </si>
+  <si>
+    <t>offshore wind resource -- CF class wof-DEU_55 -- cost class 1</t>
+  </si>
+  <si>
+    <t>e_wof-DEU_54_c1</t>
+  </si>
+  <si>
+    <t>offshore wind resource -- CF class wof-DEU_54 -- cost class 1</t>
+  </si>
+  <si>
+    <t>e_wof-DEU_53_c2</t>
+  </si>
+  <si>
+    <t>offshore wind resource -- CF class wof-DEU_53 -- cost class 2</t>
+  </si>
+  <si>
+    <t>e_wof-DEU_53_c1</t>
+  </si>
+  <si>
+    <t>offshore wind resource -- CF class wof-DEU_53 -- cost class 1</t>
+  </si>
+  <si>
+    <t>e_wof-DEU_52_c1</t>
+  </si>
+  <si>
+    <t>offshore wind resource -- CF class wof-DEU_52 -- cost class 1</t>
+  </si>
+  <si>
+    <t>e_wof-DEU_52_c2</t>
+  </si>
+  <si>
+    <t>offshore wind resource -- CF class wof-DEU_52 -- cost class 2</t>
+  </si>
+  <si>
+    <t>e_wof-DEU_49_c2</t>
+  </si>
+  <si>
+    <t>offshore wind resource -- CF class wof-DEU_49 -- cost class 2</t>
+  </si>
+  <si>
+    <t>e_wof-DEU_49_c1</t>
+  </si>
+  <si>
+    <t>offshore wind resource -- CF class wof-DEU_49 -- cost class 1</t>
+  </si>
+  <si>
+    <t>e_wof-DEU_48_c1</t>
+  </si>
+  <si>
+    <t>offshore wind resource -- CF class wof-DEU_48 -- cost class 1</t>
+  </si>
+  <si>
+    <t>e_wof-DEU_46_c1</t>
+  </si>
+  <si>
+    <t>offshore wind resource -- CF class wof-DEU_46 -- cost class 1</t>
+  </si>
+  <si>
+    <t>e_wof-DEU_46_c2</t>
+  </si>
+  <si>
+    <t>offshore wind resource -- CF class wof-DEU_46 -- cost class 2</t>
+  </si>
+  <si>
+    <t>e_wof-DEU_44_c1</t>
+  </si>
+  <si>
+    <t>offshore wind resource -- CF class wof-DEU_44 -- cost class 1</t>
+  </si>
+  <si>
+    <t>e_wof-DEU_43_c1</t>
+  </si>
+  <si>
+    <t>offshore wind resource -- CF class wof-DEU_43 -- cost class 1</t>
+  </si>
+  <si>
+    <t>e_wof-DEU_42_c1</t>
+  </si>
+  <si>
+    <t>offshore wind resource -- CF class wof-DEU_42 -- cost class 1</t>
+  </si>
+  <si>
+    <t>e_wof-DEU_40_c1</t>
+  </si>
+  <si>
+    <t>offshore wind resource -- CF class wof-DEU_40 -- cost class 1</t>
+  </si>
+  <si>
+    <t>e_wof-DEU_39_c1</t>
+  </si>
+  <si>
+    <t>offshore wind resource -- CF class wof-DEU_39 -- cost class 1</t>
+  </si>
+  <si>
+    <t>e_wof-DEU_39_c2</t>
+  </si>
+  <si>
+    <t>offshore wind resource -- CF class wof-DEU_39 -- cost class 2</t>
+  </si>
+  <si>
+    <t>e_wof-DEU_36_c2</t>
+  </si>
+  <si>
+    <t>offshore wind resource -- CF class wof-DEU_36 -- cost class 2</t>
+  </si>
+  <si>
+    <t>e_wof-DEU_36_c1</t>
+  </si>
+  <si>
+    <t>offshore wind resource -- CF class wof-DEU_36 -- cost class 1</t>
+  </si>
+  <si>
+    <t>e_wof-DEU_35_c1</t>
+  </si>
+  <si>
+    <t>offshore wind resource -- CF class wof-DEU_35 -- cost class 1</t>
+  </si>
+  <si>
+    <t>e_wof-DEU_34_c2</t>
+  </si>
+  <si>
+    <t>offshore wind resource -- CF class wof-DEU_34 -- cost class 2</t>
+  </si>
+  <si>
+    <t>e_wof-DEU_34_c1</t>
+  </si>
+  <si>
+    <t>offshore wind resource -- CF class wof-DEU_34 -- cost class 1</t>
+  </si>
+  <si>
+    <t>e_wof-DEU_31_c1</t>
+  </si>
+  <si>
+    <t>offshore wind resource -- CF class wof-DEU_31 -- cost class 1</t>
+  </si>
+  <si>
+    <t>e_wof-DEU_30_c1</t>
+  </si>
+  <si>
+    <t>offshore wind resource -- CF class wof-DEU_30 -- cost class 1</t>
+  </si>
+  <si>
+    <t>e_wof-DEU_29_c1</t>
+  </si>
+  <si>
+    <t>offshore wind resource -- CF class wof-DEU_29 -- cost class 1</t>
+  </si>
+  <si>
+    <t>elc_wof-DEU</t>
   </si>
   <si>
     <t>comm-in</t>
@@ -2800,7 +3019,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4BC1A71-01B8-2DD8-EDD3-4B012ECA05B5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{580E2BD9-B885-6EE0-BDCD-45052E27766A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2855,7 +3074,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{841538BC-84BC-E047-9653-B43CFCF71A49}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43FABB0C-987F-6E33-35AA-8BF5267D8504}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2910,7 +3129,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{478BE0AC-5ED6-23DB-6F54-D92980CA32C8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1F4CA59-85F2-E984-96A9-0E244ABE5476}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2965,7 +3184,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B417802-957C-3FE6-B4D9-CE2AF4B17E99}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46FD4F18-AF89-1422-04AA-C4CC8C12F9FF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6895,7 +7114,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7CECAE9-2946-4E0D-A22C-4A8821927575}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD8905F6-3653-4930-97B5-EB6447F2C35D}">
   <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7972,8 +8191,8 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2A337A4-2075-4AAC-B13C-54F688CDC3E1}">
-  <dimension ref="A1:O154"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899E3FFA-71C8-40E0-BF81-6954D2208FCA}">
+  <dimension ref="A1:AC154"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
@@ -7992,9 +8211,18 @@
     <col min="11" max="13" width="10.59765625" customWidth="1"/>
     <col min="14" max="14" width="19.265625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.59765625" customWidth="1"/>
+    <col min="17" max="17" width="10.59765625" customWidth="1"/>
+    <col min="18" max="18" width="13.265625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="30.59765625" customWidth="1"/>
+    <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.46484375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.59765625" customWidth="1"/>
+    <col min="25" max="25" width="13.265625" bestFit="1" customWidth="1"/>
+    <col min="26" max="29" width="10.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="22.05" customHeight="1">
+    <row r="1" spans="1:29" ht="22.05" customHeight="1">
       <c r="A1" s="153" t="s">
         <v>163</v>
       </c>
@@ -8006,15 +8234,21 @@
       <c r="G1" s="153"/>
       <c r="H1" s="153"/>
     </row>
-    <row r="9" spans="1:15" ht="14.65" thickBot="1">
+    <row r="9" spans="1:29" ht="14.65" thickBot="1">
       <c r="B9" s="154" t="s">
         <v>152</v>
       </c>
       <c r="J9" s="154" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" ht="15.75" thickBot="1">
+      <c r="Q9" s="154" t="s">
+        <v>152</v>
+      </c>
+      <c r="Y9" s="154" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" ht="15.75" thickBot="1">
       <c r="B10" s="155" t="s">
         <v>168</v>
       </c>
@@ -8054,8 +8288,44 @@
       <c r="O10" s="155" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="11" spans="1:15">
+      <c r="Q10" s="155" t="s">
+        <v>168</v>
+      </c>
+      <c r="R10" s="155" t="s">
+        <v>153</v>
+      </c>
+      <c r="S10" s="155" t="s">
+        <v>154</v>
+      </c>
+      <c r="T10" s="155" t="s">
+        <v>169</v>
+      </c>
+      <c r="U10" s="155" t="s">
+        <v>170</v>
+      </c>
+      <c r="V10" s="155" t="s">
+        <v>155</v>
+      </c>
+      <c r="W10" s="155" t="s">
+        <v>171</v>
+      </c>
+      <c r="Y10" s="155" t="s">
+        <v>153</v>
+      </c>
+      <c r="Z10" s="155" t="s">
+        <v>223</v>
+      </c>
+      <c r="AA10" s="155" t="s">
+        <v>224</v>
+      </c>
+      <c r="AB10" s="155" t="s">
+        <v>225</v>
+      </c>
+      <c r="AC10" s="155" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29">
       <c r="B11" s="156" t="s">
         <v>172</v>
       </c>
@@ -8095,8 +8365,44 @@
       <c r="O11" s="158">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:15">
+      <c r="Q11" s="156" t="s">
+        <v>172</v>
+      </c>
+      <c r="R11" s="156" t="s">
+        <v>518</v>
+      </c>
+      <c r="S11" s="156" t="s">
+        <v>519</v>
+      </c>
+      <c r="T11" s="156" t="s">
+        <v>10</v>
+      </c>
+      <c r="U11" s="156" t="s">
+        <v>21</v>
+      </c>
+      <c r="V11" s="156" t="s">
+        <v>175</v>
+      </c>
+      <c r="W11" s="156" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y11" s="156" t="s">
+        <v>518</v>
+      </c>
+      <c r="Z11" s="156" t="s">
+        <v>590</v>
+      </c>
+      <c r="AA11" s="158">
+        <v>13.8675</v>
+      </c>
+      <c r="AB11" s="161">
+        <v>0.59497267100000006</v>
+      </c>
+      <c r="AC11" s="158">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29">
       <c r="B12" s="157" t="s">
         <v>172</v>
       </c>
@@ -8136,8 +8442,44 @@
       <c r="O12" s="159">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:15">
+      <c r="Q12" s="157" t="s">
+        <v>172</v>
+      </c>
+      <c r="R12" s="157" t="s">
+        <v>520</v>
+      </c>
+      <c r="S12" s="157" t="s">
+        <v>521</v>
+      </c>
+      <c r="T12" s="157" t="s">
+        <v>10</v>
+      </c>
+      <c r="U12" s="157" t="s">
+        <v>21</v>
+      </c>
+      <c r="V12" s="157" t="s">
+        <v>175</v>
+      </c>
+      <c r="W12" s="157" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y12" s="157" t="s">
+        <v>520</v>
+      </c>
+      <c r="Z12" s="157" t="s">
+        <v>590</v>
+      </c>
+      <c r="AA12" s="159">
+        <v>11.755000000000001</v>
+      </c>
+      <c r="AB12" s="163">
+        <v>0.59425257200000003</v>
+      </c>
+      <c r="AC12" s="159">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29">
       <c r="B13" s="156" t="s">
         <v>172</v>
       </c>
@@ -8177,8 +8519,44 @@
       <c r="O13" s="158">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:15">
+      <c r="Q13" s="156" t="s">
+        <v>172</v>
+      </c>
+      <c r="R13" s="156" t="s">
+        <v>522</v>
+      </c>
+      <c r="S13" s="156" t="s">
+        <v>523</v>
+      </c>
+      <c r="T13" s="156" t="s">
+        <v>10</v>
+      </c>
+      <c r="U13" s="156" t="s">
+        <v>21</v>
+      </c>
+      <c r="V13" s="156" t="s">
+        <v>175</v>
+      </c>
+      <c r="W13" s="156" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y13" s="156" t="s">
+        <v>522</v>
+      </c>
+      <c r="Z13" s="156" t="s">
+        <v>590</v>
+      </c>
+      <c r="AA13" s="158">
+        <v>27.734999999999999</v>
+      </c>
+      <c r="AB13" s="161">
+        <v>0.59103745399999996</v>
+      </c>
+      <c r="AC13" s="158">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29">
       <c r="B14" s="157" t="s">
         <v>172</v>
       </c>
@@ -8218,8 +8596,44 @@
       <c r="O14" s="159">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:15">
+      <c r="Q14" s="157" t="s">
+        <v>172</v>
+      </c>
+      <c r="R14" s="157" t="s">
+        <v>524</v>
+      </c>
+      <c r="S14" s="157" t="s">
+        <v>525</v>
+      </c>
+      <c r="T14" s="157" t="s">
+        <v>10</v>
+      </c>
+      <c r="U14" s="157" t="s">
+        <v>21</v>
+      </c>
+      <c r="V14" s="157" t="s">
+        <v>175</v>
+      </c>
+      <c r="W14" s="157" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y14" s="157" t="s">
+        <v>524</v>
+      </c>
+      <c r="Z14" s="157" t="s">
+        <v>590</v>
+      </c>
+      <c r="AA14" s="159">
+        <v>13.8675</v>
+      </c>
+      <c r="AB14" s="163">
+        <v>0.58995215400000001</v>
+      </c>
+      <c r="AC14" s="159">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29">
       <c r="B15" s="156" t="s">
         <v>172</v>
       </c>
@@ -8259,8 +8673,44 @@
       <c r="O15" s="158">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:15">
+      <c r="Q15" s="156" t="s">
+        <v>172</v>
+      </c>
+      <c r="R15" s="156" t="s">
+        <v>526</v>
+      </c>
+      <c r="S15" s="156" t="s">
+        <v>527</v>
+      </c>
+      <c r="T15" s="156" t="s">
+        <v>10</v>
+      </c>
+      <c r="U15" s="156" t="s">
+        <v>21</v>
+      </c>
+      <c r="V15" s="156" t="s">
+        <v>175</v>
+      </c>
+      <c r="W15" s="156" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y15" s="156" t="s">
+        <v>526</v>
+      </c>
+      <c r="Z15" s="156" t="s">
+        <v>590</v>
+      </c>
+      <c r="AA15" s="158">
+        <v>27.734999999999999</v>
+      </c>
+      <c r="AB15" s="161">
+        <v>0.58755964500000002</v>
+      </c>
+      <c r="AC15" s="158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29">
       <c r="B16" s="157" t="s">
         <v>172</v>
       </c>
@@ -8300,8 +8750,44 @@
       <c r="O16" s="159">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="2:15">
+      <c r="Q16" s="157" t="s">
+        <v>172</v>
+      </c>
+      <c r="R16" s="157" t="s">
+        <v>528</v>
+      </c>
+      <c r="S16" s="157" t="s">
+        <v>529</v>
+      </c>
+      <c r="T16" s="157" t="s">
+        <v>10</v>
+      </c>
+      <c r="U16" s="157" t="s">
+        <v>21</v>
+      </c>
+      <c r="V16" s="157" t="s">
+        <v>175</v>
+      </c>
+      <c r="W16" s="157" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y16" s="157" t="s">
+        <v>528</v>
+      </c>
+      <c r="Z16" s="157" t="s">
+        <v>590</v>
+      </c>
+      <c r="AA16" s="159">
+        <v>13.8675</v>
+      </c>
+      <c r="AB16" s="163">
+        <v>0.58303503899999998</v>
+      </c>
+      <c r="AC16" s="159">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:29">
       <c r="B17" s="156" t="s">
         <v>172</v>
       </c>
@@ -8341,8 +8827,44 @@
       <c r="O17" s="158">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="2:15">
+      <c r="Q17" s="156" t="s">
+        <v>172</v>
+      </c>
+      <c r="R17" s="156" t="s">
+        <v>530</v>
+      </c>
+      <c r="S17" s="156" t="s">
+        <v>531</v>
+      </c>
+      <c r="T17" s="156" t="s">
+        <v>10</v>
+      </c>
+      <c r="U17" s="156" t="s">
+        <v>21</v>
+      </c>
+      <c r="V17" s="156" t="s">
+        <v>175</v>
+      </c>
+      <c r="W17" s="156" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y17" s="156" t="s">
+        <v>530</v>
+      </c>
+      <c r="Z17" s="156" t="s">
+        <v>590</v>
+      </c>
+      <c r="AA17" s="158">
+        <v>14.02875</v>
+      </c>
+      <c r="AB17" s="161">
+        <v>0.57868857299999998</v>
+      </c>
+      <c r="AC17" s="158">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:29">
       <c r="B18" s="157" t="s">
         <v>172</v>
       </c>
@@ -8382,8 +8904,44 @@
       <c r="O18" s="159">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="2:15">
+      <c r="Q18" s="157" t="s">
+        <v>172</v>
+      </c>
+      <c r="R18" s="157" t="s">
+        <v>532</v>
+      </c>
+      <c r="S18" s="157" t="s">
+        <v>533</v>
+      </c>
+      <c r="T18" s="157" t="s">
+        <v>10</v>
+      </c>
+      <c r="U18" s="157" t="s">
+        <v>21</v>
+      </c>
+      <c r="V18" s="157" t="s">
+        <v>175</v>
+      </c>
+      <c r="W18" s="157" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y18" s="157" t="s">
+        <v>532</v>
+      </c>
+      <c r="Z18" s="157" t="s">
+        <v>590</v>
+      </c>
+      <c r="AA18" s="159">
+        <v>13.8675</v>
+      </c>
+      <c r="AB18" s="163">
+        <v>0.57695094899999999</v>
+      </c>
+      <c r="AC18" s="159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:29">
       <c r="B19" s="156" t="s">
         <v>172</v>
       </c>
@@ -8423,8 +8981,44 @@
       <c r="O19" s="158">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="2:15">
+      <c r="Q19" s="156" t="s">
+        <v>172</v>
+      </c>
+      <c r="R19" s="156" t="s">
+        <v>534</v>
+      </c>
+      <c r="S19" s="156" t="s">
+        <v>535</v>
+      </c>
+      <c r="T19" s="156" t="s">
+        <v>10</v>
+      </c>
+      <c r="U19" s="156" t="s">
+        <v>21</v>
+      </c>
+      <c r="V19" s="156" t="s">
+        <v>175</v>
+      </c>
+      <c r="W19" s="156" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y19" s="156" t="s">
+        <v>534</v>
+      </c>
+      <c r="Z19" s="156" t="s">
+        <v>590</v>
+      </c>
+      <c r="AA19" s="158">
+        <v>14.02875</v>
+      </c>
+      <c r="AB19" s="161">
+        <v>0.57442702300000004</v>
+      </c>
+      <c r="AC19" s="158">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:29">
       <c r="B20" s="157" t="s">
         <v>172</v>
       </c>
@@ -8464,8 +9058,44 @@
       <c r="O20" s="159">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="2:15">
+      <c r="Q20" s="157" t="s">
+        <v>172</v>
+      </c>
+      <c r="R20" s="157" t="s">
+        <v>536</v>
+      </c>
+      <c r="S20" s="157" t="s">
+        <v>537</v>
+      </c>
+      <c r="T20" s="157" t="s">
+        <v>10</v>
+      </c>
+      <c r="U20" s="157" t="s">
+        <v>21</v>
+      </c>
+      <c r="V20" s="157" t="s">
+        <v>175</v>
+      </c>
+      <c r="W20" s="157" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y20" s="157" t="s">
+        <v>536</v>
+      </c>
+      <c r="Z20" s="157" t="s">
+        <v>590</v>
+      </c>
+      <c r="AA20" s="159">
+        <v>13.827500000000001</v>
+      </c>
+      <c r="AB20" s="163">
+        <v>0.57279671099999996</v>
+      </c>
+      <c r="AC20" s="159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:29">
       <c r="B21" s="156" t="s">
         <v>172</v>
       </c>
@@ -8505,8 +9135,44 @@
       <c r="O21" s="158">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="2:15">
+      <c r="Q21" s="156" t="s">
+        <v>172</v>
+      </c>
+      <c r="R21" s="156" t="s">
+        <v>538</v>
+      </c>
+      <c r="S21" s="156" t="s">
+        <v>539</v>
+      </c>
+      <c r="T21" s="156" t="s">
+        <v>10</v>
+      </c>
+      <c r="U21" s="156" t="s">
+        <v>21</v>
+      </c>
+      <c r="V21" s="156" t="s">
+        <v>175</v>
+      </c>
+      <c r="W21" s="156" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y21" s="156" t="s">
+        <v>538</v>
+      </c>
+      <c r="Z21" s="156" t="s">
+        <v>590</v>
+      </c>
+      <c r="AA21" s="158">
+        <v>13.92625</v>
+      </c>
+      <c r="AB21" s="161">
+        <v>0.56071739600000003</v>
+      </c>
+      <c r="AC21" s="158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:29">
       <c r="B22" s="157" t="s">
         <v>172</v>
       </c>
@@ -8546,8 +9212,44 @@
       <c r="O22" s="159">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="2:15">
+      <c r="Q22" s="157" t="s">
+        <v>172</v>
+      </c>
+      <c r="R22" s="157" t="s">
+        <v>540</v>
+      </c>
+      <c r="S22" s="157" t="s">
+        <v>541</v>
+      </c>
+      <c r="T22" s="157" t="s">
+        <v>10</v>
+      </c>
+      <c r="U22" s="157" t="s">
+        <v>21</v>
+      </c>
+      <c r="V22" s="157" t="s">
+        <v>175</v>
+      </c>
+      <c r="W22" s="157" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y22" s="157" t="s">
+        <v>540</v>
+      </c>
+      <c r="Z22" s="157" t="s">
+        <v>590</v>
+      </c>
+      <c r="AA22" s="159">
+        <v>13.23875</v>
+      </c>
+      <c r="AB22" s="163">
+        <v>0.553779154</v>
+      </c>
+      <c r="AC22" s="159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:29">
       <c r="B23" s="156" t="s">
         <v>172</v>
       </c>
@@ -8587,8 +9289,44 @@
       <c r="O23" s="158">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="2:15">
+      <c r="Q23" s="156" t="s">
+        <v>172</v>
+      </c>
+      <c r="R23" s="156" t="s">
+        <v>542</v>
+      </c>
+      <c r="S23" s="156" t="s">
+        <v>543</v>
+      </c>
+      <c r="T23" s="156" t="s">
+        <v>10</v>
+      </c>
+      <c r="U23" s="156" t="s">
+        <v>21</v>
+      </c>
+      <c r="V23" s="156" t="s">
+        <v>175</v>
+      </c>
+      <c r="W23" s="156" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y23" s="156" t="s">
+        <v>542</v>
+      </c>
+      <c r="Z23" s="156" t="s">
+        <v>590</v>
+      </c>
+      <c r="AA23" s="158">
+        <v>4.5162500000000003</v>
+      </c>
+      <c r="AB23" s="161">
+        <v>0.54469198200000002</v>
+      </c>
+      <c r="AC23" s="158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:29">
       <c r="B24" s="157" t="s">
         <v>172</v>
       </c>
@@ -8628,8 +9366,44 @@
       <c r="O24" s="159">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="2:15">
+      <c r="Q24" s="157" t="s">
+        <v>172</v>
+      </c>
+      <c r="R24" s="157" t="s">
+        <v>544</v>
+      </c>
+      <c r="S24" s="157" t="s">
+        <v>545</v>
+      </c>
+      <c r="T24" s="157" t="s">
+        <v>10</v>
+      </c>
+      <c r="U24" s="157" t="s">
+        <v>21</v>
+      </c>
+      <c r="V24" s="157" t="s">
+        <v>175</v>
+      </c>
+      <c r="W24" s="157" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y24" s="157" t="s">
+        <v>544</v>
+      </c>
+      <c r="Z24" s="157" t="s">
+        <v>590</v>
+      </c>
+      <c r="AA24" s="159">
+        <v>13.8675</v>
+      </c>
+      <c r="AB24" s="163">
+        <v>0.53262292899999997</v>
+      </c>
+      <c r="AC24" s="159">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:29">
       <c r="B25" s="156" t="s">
         <v>172</v>
       </c>
@@ -8669,8 +9443,44 @@
       <c r="O25" s="158">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="2:15">
+      <c r="Q25" s="156" t="s">
+        <v>172</v>
+      </c>
+      <c r="R25" s="156" t="s">
+        <v>546</v>
+      </c>
+      <c r="S25" s="156" t="s">
+        <v>547</v>
+      </c>
+      <c r="T25" s="156" t="s">
+        <v>10</v>
+      </c>
+      <c r="U25" s="156" t="s">
+        <v>21</v>
+      </c>
+      <c r="V25" s="156" t="s">
+        <v>175</v>
+      </c>
+      <c r="W25" s="156" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y25" s="156" t="s">
+        <v>546</v>
+      </c>
+      <c r="Z25" s="156" t="s">
+        <v>590</v>
+      </c>
+      <c r="AA25" s="158">
+        <v>8.1549999999999994</v>
+      </c>
+      <c r="AB25" s="161">
+        <v>0.53167315900000001</v>
+      </c>
+      <c r="AC25" s="158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:29">
       <c r="B26" s="157" t="s">
         <v>172</v>
       </c>
@@ -8710,8 +9520,44 @@
       <c r="O26" s="159">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="2:15">
+      <c r="Q26" s="157" t="s">
+        <v>172</v>
+      </c>
+      <c r="R26" s="157" t="s">
+        <v>548</v>
+      </c>
+      <c r="S26" s="157" t="s">
+        <v>549</v>
+      </c>
+      <c r="T26" s="157" t="s">
+        <v>10</v>
+      </c>
+      <c r="U26" s="157" t="s">
+        <v>21</v>
+      </c>
+      <c r="V26" s="157" t="s">
+        <v>175</v>
+      </c>
+      <c r="W26" s="157" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y26" s="157" t="s">
+        <v>548</v>
+      </c>
+      <c r="Z26" s="157" t="s">
+        <v>590</v>
+      </c>
+      <c r="AA26" s="159">
+        <v>9.06</v>
+      </c>
+      <c r="AB26" s="163">
+        <v>0.52457923100000003</v>
+      </c>
+      <c r="AC26" s="159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:29">
       <c r="B27" s="156" t="s">
         <v>172</v>
       </c>
@@ -8751,8 +9597,44 @@
       <c r="O27" s="158">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="2:15">
+      <c r="Q27" s="156" t="s">
+        <v>172</v>
+      </c>
+      <c r="R27" s="156" t="s">
+        <v>550</v>
+      </c>
+      <c r="S27" s="156" t="s">
+        <v>551</v>
+      </c>
+      <c r="T27" s="156" t="s">
+        <v>10</v>
+      </c>
+      <c r="U27" s="156" t="s">
+        <v>21</v>
+      </c>
+      <c r="V27" s="156" t="s">
+        <v>175</v>
+      </c>
+      <c r="W27" s="156" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y27" s="156" t="s">
+        <v>550</v>
+      </c>
+      <c r="Z27" s="156" t="s">
+        <v>590</v>
+      </c>
+      <c r="AA27" s="158">
+        <v>11.2575</v>
+      </c>
+      <c r="AB27" s="161">
+        <v>0.51877992900000003</v>
+      </c>
+      <c r="AC27" s="158">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:29">
       <c r="B28" s="157" t="s">
         <v>172</v>
       </c>
@@ -8792,8 +9674,44 @@
       <c r="O28" s="159">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="2:15">
+      <c r="Q28" s="157" t="s">
+        <v>172</v>
+      </c>
+      <c r="R28" s="157" t="s">
+        <v>552</v>
+      </c>
+      <c r="S28" s="157" t="s">
+        <v>553</v>
+      </c>
+      <c r="T28" s="157" t="s">
+        <v>10</v>
+      </c>
+      <c r="U28" s="157" t="s">
+        <v>21</v>
+      </c>
+      <c r="V28" s="157" t="s">
+        <v>175</v>
+      </c>
+      <c r="W28" s="157" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y28" s="157" t="s">
+        <v>552</v>
+      </c>
+      <c r="Z28" s="157" t="s">
+        <v>590</v>
+      </c>
+      <c r="AA28" s="159">
+        <v>10.8575</v>
+      </c>
+      <c r="AB28" s="163">
+        <v>0.49296379099999993</v>
+      </c>
+      <c r="AC28" s="159">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:29">
       <c r="B29" s="156" t="s">
         <v>172</v>
       </c>
@@ -8833,8 +9751,44 @@
       <c r="O29" s="158">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="2:15">
+      <c r="Q29" s="156" t="s">
+        <v>172</v>
+      </c>
+      <c r="R29" s="156" t="s">
+        <v>554</v>
+      </c>
+      <c r="S29" s="156" t="s">
+        <v>555</v>
+      </c>
+      <c r="T29" s="156" t="s">
+        <v>10</v>
+      </c>
+      <c r="U29" s="156" t="s">
+        <v>21</v>
+      </c>
+      <c r="V29" s="156" t="s">
+        <v>175</v>
+      </c>
+      <c r="W29" s="156" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y29" s="156" t="s">
+        <v>554</v>
+      </c>
+      <c r="Z29" s="156" t="s">
+        <v>590</v>
+      </c>
+      <c r="AA29" s="158">
+        <v>6.6375000000000002</v>
+      </c>
+      <c r="AB29" s="161">
+        <v>0.48683053799999998</v>
+      </c>
+      <c r="AC29" s="158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:29">
       <c r="B30" s="157" t="s">
         <v>172</v>
       </c>
@@ -8874,8 +9828,44 @@
       <c r="O30" s="159">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="2:15">
+      <c r="Q30" s="157" t="s">
+        <v>172</v>
+      </c>
+      <c r="R30" s="157" t="s">
+        <v>556</v>
+      </c>
+      <c r="S30" s="157" t="s">
+        <v>557</v>
+      </c>
+      <c r="T30" s="157" t="s">
+        <v>10</v>
+      </c>
+      <c r="U30" s="157" t="s">
+        <v>21</v>
+      </c>
+      <c r="V30" s="157" t="s">
+        <v>175</v>
+      </c>
+      <c r="W30" s="157" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y30" s="157" t="s">
+        <v>556</v>
+      </c>
+      <c r="Z30" s="157" t="s">
+        <v>590</v>
+      </c>
+      <c r="AA30" s="159">
+        <v>12.063750000000001</v>
+      </c>
+      <c r="AB30" s="163">
+        <v>0.47927646499999998</v>
+      </c>
+      <c r="AC30" s="159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:29">
       <c r="B31" s="156" t="s">
         <v>172</v>
       </c>
@@ -8915,8 +9905,44 @@
       <c r="O31" s="158">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="2:15">
+      <c r="Q31" s="156" t="s">
+        <v>172</v>
+      </c>
+      <c r="R31" s="156" t="s">
+        <v>558</v>
+      </c>
+      <c r="S31" s="156" t="s">
+        <v>559</v>
+      </c>
+      <c r="T31" s="156" t="s">
+        <v>10</v>
+      </c>
+      <c r="U31" s="156" t="s">
+        <v>21</v>
+      </c>
+      <c r="V31" s="156" t="s">
+        <v>175</v>
+      </c>
+      <c r="W31" s="156" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y31" s="156" t="s">
+        <v>558</v>
+      </c>
+      <c r="Z31" s="156" t="s">
+        <v>590</v>
+      </c>
+      <c r="AA31" s="158">
+        <v>0.11874999999999999</v>
+      </c>
+      <c r="AB31" s="161">
+        <v>0.46083247599999999</v>
+      </c>
+      <c r="AC31" s="158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:29">
       <c r="B32" s="157" t="s">
         <v>172</v>
       </c>
@@ -8956,8 +9982,44 @@
       <c r="O32" s="159">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="2:15">
+      <c r="Q32" s="157" t="s">
+        <v>172</v>
+      </c>
+      <c r="R32" s="157" t="s">
+        <v>560</v>
+      </c>
+      <c r="S32" s="157" t="s">
+        <v>561</v>
+      </c>
+      <c r="T32" s="157" t="s">
+        <v>10</v>
+      </c>
+      <c r="U32" s="157" t="s">
+        <v>21</v>
+      </c>
+      <c r="V32" s="157" t="s">
+        <v>175</v>
+      </c>
+      <c r="W32" s="157" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y32" s="157" t="s">
+        <v>560</v>
+      </c>
+      <c r="Z32" s="157" t="s">
+        <v>590</v>
+      </c>
+      <c r="AA32" s="159">
+        <v>2.8424999999999998</v>
+      </c>
+      <c r="AB32" s="163">
+        <v>0.45533161299999997</v>
+      </c>
+      <c r="AC32" s="159">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:29">
       <c r="B33" s="156" t="s">
         <v>172</v>
       </c>
@@ -8997,8 +10059,44 @@
       <c r="O33" s="158">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="2:15">
+      <c r="Q33" s="156" t="s">
+        <v>172</v>
+      </c>
+      <c r="R33" s="156" t="s">
+        <v>562</v>
+      </c>
+      <c r="S33" s="156" t="s">
+        <v>563</v>
+      </c>
+      <c r="T33" s="156" t="s">
+        <v>10</v>
+      </c>
+      <c r="U33" s="156" t="s">
+        <v>21</v>
+      </c>
+      <c r="V33" s="156" t="s">
+        <v>175</v>
+      </c>
+      <c r="W33" s="156" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y33" s="156" t="s">
+        <v>562</v>
+      </c>
+      <c r="Z33" s="156" t="s">
+        <v>590</v>
+      </c>
+      <c r="AA33" s="158">
+        <v>10.682499999999999</v>
+      </c>
+      <c r="AB33" s="161">
+        <v>0.43737909600000002</v>
+      </c>
+      <c r="AC33" s="158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:29">
       <c r="B34" s="157" t="s">
         <v>172</v>
       </c>
@@ -9038,8 +10136,44 @@
       <c r="O34" s="159">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="2:15">
+      <c r="Q34" s="157" t="s">
+        <v>172</v>
+      </c>
+      <c r="R34" s="157" t="s">
+        <v>564</v>
+      </c>
+      <c r="S34" s="157" t="s">
+        <v>565</v>
+      </c>
+      <c r="T34" s="157" t="s">
+        <v>10</v>
+      </c>
+      <c r="U34" s="157" t="s">
+        <v>21</v>
+      </c>
+      <c r="V34" s="157" t="s">
+        <v>175</v>
+      </c>
+      <c r="W34" s="157" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y34" s="157" t="s">
+        <v>564</v>
+      </c>
+      <c r="Z34" s="157" t="s">
+        <v>590</v>
+      </c>
+      <c r="AA34" s="159">
+        <v>5.9212499999999997</v>
+      </c>
+      <c r="AB34" s="163">
+        <v>0.43435844699999998</v>
+      </c>
+      <c r="AC34" s="159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:29">
       <c r="B35" s="156" t="s">
         <v>172</v>
       </c>
@@ -9079,8 +10213,44 @@
       <c r="O35" s="158">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="2:15">
+      <c r="Q35" s="156" t="s">
+        <v>172</v>
+      </c>
+      <c r="R35" s="156" t="s">
+        <v>566</v>
+      </c>
+      <c r="S35" s="156" t="s">
+        <v>567</v>
+      </c>
+      <c r="T35" s="156" t="s">
+        <v>10</v>
+      </c>
+      <c r="U35" s="156" t="s">
+        <v>21</v>
+      </c>
+      <c r="V35" s="156" t="s">
+        <v>175</v>
+      </c>
+      <c r="W35" s="156" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y35" s="156" t="s">
+        <v>566</v>
+      </c>
+      <c r="Z35" s="156" t="s">
+        <v>590</v>
+      </c>
+      <c r="AA35" s="158">
+        <v>2.61375</v>
+      </c>
+      <c r="AB35" s="161">
+        <v>0.42359337499999994</v>
+      </c>
+      <c r="AC35" s="158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:29">
       <c r="B36" s="157" t="s">
         <v>172</v>
       </c>
@@ -9120,8 +10290,44 @@
       <c r="O36" s="159">
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="2:15">
+      <c r="Q36" s="157" t="s">
+        <v>172</v>
+      </c>
+      <c r="R36" s="157" t="s">
+        <v>568</v>
+      </c>
+      <c r="S36" s="157" t="s">
+        <v>569</v>
+      </c>
+      <c r="T36" s="157" t="s">
+        <v>10</v>
+      </c>
+      <c r="U36" s="157" t="s">
+        <v>21</v>
+      </c>
+      <c r="V36" s="157" t="s">
+        <v>175</v>
+      </c>
+      <c r="W36" s="157" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y36" s="157" t="s">
+        <v>568</v>
+      </c>
+      <c r="Z36" s="157" t="s">
+        <v>590</v>
+      </c>
+      <c r="AA36" s="159">
+        <v>3.9175</v>
+      </c>
+      <c r="AB36" s="163">
+        <v>0.402605345</v>
+      </c>
+      <c r="AC36" s="159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:29">
       <c r="B37" s="156" t="s">
         <v>172</v>
       </c>
@@ -9161,8 +10367,44 @@
       <c r="O37" s="158">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="2:15">
+      <c r="Q37" s="156" t="s">
+        <v>172</v>
+      </c>
+      <c r="R37" s="156" t="s">
+        <v>570</v>
+      </c>
+      <c r="S37" s="156" t="s">
+        <v>571</v>
+      </c>
+      <c r="T37" s="156" t="s">
+        <v>10</v>
+      </c>
+      <c r="U37" s="156" t="s">
+        <v>21</v>
+      </c>
+      <c r="V37" s="156" t="s">
+        <v>175</v>
+      </c>
+      <c r="W37" s="156" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y37" s="156" t="s">
+        <v>570</v>
+      </c>
+      <c r="Z37" s="156" t="s">
+        <v>590</v>
+      </c>
+      <c r="AA37" s="158">
+        <v>1.0075000000000001</v>
+      </c>
+      <c r="AB37" s="161">
+        <v>0.39005562999999999</v>
+      </c>
+      <c r="AC37" s="158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:29">
       <c r="B38" s="157" t="s">
         <v>172</v>
       </c>
@@ -9202,8 +10444,44 @@
       <c r="O38" s="159">
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="2:15">
+      <c r="Q38" s="157" t="s">
+        <v>172</v>
+      </c>
+      <c r="R38" s="157" t="s">
+        <v>572</v>
+      </c>
+      <c r="S38" s="157" t="s">
+        <v>573</v>
+      </c>
+      <c r="T38" s="157" t="s">
+        <v>10</v>
+      </c>
+      <c r="U38" s="157" t="s">
+        <v>21</v>
+      </c>
+      <c r="V38" s="157" t="s">
+        <v>175</v>
+      </c>
+      <c r="W38" s="157" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y38" s="157" t="s">
+        <v>572</v>
+      </c>
+      <c r="Z38" s="157" t="s">
+        <v>590</v>
+      </c>
+      <c r="AA38" s="159">
+        <v>0.58250000000000002</v>
+      </c>
+      <c r="AB38" s="163">
+        <v>0.38518730299999998</v>
+      </c>
+      <c r="AC38" s="159">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:29">
       <c r="B39" s="156" t="s">
         <v>172</v>
       </c>
@@ -9243,8 +10521,44 @@
       <c r="O39" s="158">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="2:15">
+      <c r="Q39" s="156" t="s">
+        <v>172</v>
+      </c>
+      <c r="R39" s="156" t="s">
+        <v>574</v>
+      </c>
+      <c r="S39" s="156" t="s">
+        <v>575</v>
+      </c>
+      <c r="T39" s="156" t="s">
+        <v>10</v>
+      </c>
+      <c r="U39" s="156" t="s">
+        <v>21</v>
+      </c>
+      <c r="V39" s="156" t="s">
+        <v>175</v>
+      </c>
+      <c r="W39" s="156" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y39" s="156" t="s">
+        <v>574</v>
+      </c>
+      <c r="Z39" s="156" t="s">
+        <v>590</v>
+      </c>
+      <c r="AA39" s="158">
+        <v>3.7499999999999999E-3</v>
+      </c>
+      <c r="AB39" s="161">
+        <v>0.36300389399999999</v>
+      </c>
+      <c r="AC39" s="158">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:29">
       <c r="B40" s="157" t="s">
         <v>172</v>
       </c>
@@ -9284,8 +10598,44 @@
       <c r="O40" s="159">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="2:15">
+      <c r="Q40" s="157" t="s">
+        <v>172</v>
+      </c>
+      <c r="R40" s="157" t="s">
+        <v>576</v>
+      </c>
+      <c r="S40" s="157" t="s">
+        <v>577</v>
+      </c>
+      <c r="T40" s="157" t="s">
+        <v>10</v>
+      </c>
+      <c r="U40" s="157" t="s">
+        <v>21</v>
+      </c>
+      <c r="V40" s="157" t="s">
+        <v>175</v>
+      </c>
+      <c r="W40" s="157" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y40" s="157" t="s">
+        <v>576</v>
+      </c>
+      <c r="Z40" s="157" t="s">
+        <v>590</v>
+      </c>
+      <c r="AA40" s="159">
+        <v>0.57625000000000004</v>
+      </c>
+      <c r="AB40" s="163">
+        <v>0.35521376900000001</v>
+      </c>
+      <c r="AC40" s="159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="2:29">
       <c r="B41" s="156" t="s">
         <v>172</v>
       </c>
@@ -9325,8 +10675,44 @@
       <c r="O41" s="158">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="2:15">
+      <c r="Q41" s="156" t="s">
+        <v>172</v>
+      </c>
+      <c r="R41" s="156" t="s">
+        <v>578</v>
+      </c>
+      <c r="S41" s="156" t="s">
+        <v>579</v>
+      </c>
+      <c r="T41" s="156" t="s">
+        <v>10</v>
+      </c>
+      <c r="U41" s="156" t="s">
+        <v>21</v>
+      </c>
+      <c r="V41" s="156" t="s">
+        <v>175</v>
+      </c>
+      <c r="W41" s="156" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y41" s="156" t="s">
+        <v>578</v>
+      </c>
+      <c r="Z41" s="156" t="s">
+        <v>590</v>
+      </c>
+      <c r="AA41" s="158">
+        <v>2.75E-2</v>
+      </c>
+      <c r="AB41" s="161">
+        <v>0.35255688199999996</v>
+      </c>
+      <c r="AC41" s="158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:29">
       <c r="B42" s="157" t="s">
         <v>172</v>
       </c>
@@ -9366,8 +10752,44 @@
       <c r="O42" s="159">
         <v>2</v>
       </c>
-    </row>
-    <row r="43" spans="2:15">
+      <c r="Q42" s="157" t="s">
+        <v>172</v>
+      </c>
+      <c r="R42" s="157" t="s">
+        <v>580</v>
+      </c>
+      <c r="S42" s="157" t="s">
+        <v>581</v>
+      </c>
+      <c r="T42" s="157" t="s">
+        <v>10</v>
+      </c>
+      <c r="U42" s="157" t="s">
+        <v>21</v>
+      </c>
+      <c r="V42" s="157" t="s">
+        <v>175</v>
+      </c>
+      <c r="W42" s="157" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y42" s="157" t="s">
+        <v>580</v>
+      </c>
+      <c r="Z42" s="157" t="s">
+        <v>590</v>
+      </c>
+      <c r="AA42" s="159">
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="AB42" s="163">
+        <v>0.34343951499999997</v>
+      </c>
+      <c r="AC42" s="159">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="2:29">
       <c r="B43" s="156" t="s">
         <v>172</v>
       </c>
@@ -9407,8 +10829,44 @@
       <c r="O43" s="158">
         <v>3</v>
       </c>
-    </row>
-    <row r="44" spans="2:15">
+      <c r="Q43" s="156" t="s">
+        <v>172</v>
+      </c>
+      <c r="R43" s="156" t="s">
+        <v>582</v>
+      </c>
+      <c r="S43" s="156" t="s">
+        <v>583</v>
+      </c>
+      <c r="T43" s="156" t="s">
+        <v>10</v>
+      </c>
+      <c r="U43" s="156" t="s">
+        <v>21</v>
+      </c>
+      <c r="V43" s="156" t="s">
+        <v>175</v>
+      </c>
+      <c r="W43" s="156" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y43" s="156" t="s">
+        <v>582</v>
+      </c>
+      <c r="Z43" s="156" t="s">
+        <v>590</v>
+      </c>
+      <c r="AA43" s="158">
+        <v>0.21625</v>
+      </c>
+      <c r="AB43" s="161">
+        <v>0.34322851199999999</v>
+      </c>
+      <c r="AC43" s="158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="2:29">
       <c r="B44" s="157" t="s">
         <v>172</v>
       </c>
@@ -9448,8 +10906,44 @@
       <c r="O44" s="159">
         <v>2</v>
       </c>
-    </row>
-    <row r="45" spans="2:15">
+      <c r="Q44" s="157" t="s">
+        <v>172</v>
+      </c>
+      <c r="R44" s="157" t="s">
+        <v>584</v>
+      </c>
+      <c r="S44" s="157" t="s">
+        <v>585</v>
+      </c>
+      <c r="T44" s="157" t="s">
+        <v>10</v>
+      </c>
+      <c r="U44" s="157" t="s">
+        <v>21</v>
+      </c>
+      <c r="V44" s="157" t="s">
+        <v>175</v>
+      </c>
+      <c r="W44" s="157" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y44" s="157" t="s">
+        <v>584</v>
+      </c>
+      <c r="Z44" s="157" t="s">
+        <v>590</v>
+      </c>
+      <c r="AA44" s="159">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="AB44" s="163">
+        <v>0.30605732200000002</v>
+      </c>
+      <c r="AC44" s="159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="2:29">
       <c r="B45" s="156" t="s">
         <v>172</v>
       </c>
@@ -9489,8 +10983,44 @@
       <c r="O45" s="158">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="2:15">
+      <c r="Q45" s="156" t="s">
+        <v>172</v>
+      </c>
+      <c r="R45" s="156" t="s">
+        <v>586</v>
+      </c>
+      <c r="S45" s="156" t="s">
+        <v>587</v>
+      </c>
+      <c r="T45" s="156" t="s">
+        <v>10</v>
+      </c>
+      <c r="U45" s="156" t="s">
+        <v>21</v>
+      </c>
+      <c r="V45" s="156" t="s">
+        <v>175</v>
+      </c>
+      <c r="W45" s="156" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y45" s="156" t="s">
+        <v>586</v>
+      </c>
+      <c r="Z45" s="156" t="s">
+        <v>590</v>
+      </c>
+      <c r="AA45" s="158">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AB45" s="161">
+        <v>0.30015657400000001</v>
+      </c>
+      <c r="AC45" s="158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:29">
       <c r="B46" s="157" t="s">
         <v>172</v>
       </c>
@@ -9530,8 +11060,44 @@
       <c r="O46" s="159">
         <v>2</v>
       </c>
-    </row>
-    <row r="47" spans="2:15">
+      <c r="Q46" s="157" t="s">
+        <v>172</v>
+      </c>
+      <c r="R46" s="157" t="s">
+        <v>588</v>
+      </c>
+      <c r="S46" s="157" t="s">
+        <v>589</v>
+      </c>
+      <c r="T46" s="157" t="s">
+        <v>10</v>
+      </c>
+      <c r="U46" s="157" t="s">
+        <v>21</v>
+      </c>
+      <c r="V46" s="157" t="s">
+        <v>175</v>
+      </c>
+      <c r="W46" s="157" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y46" s="157" t="s">
+        <v>588</v>
+      </c>
+      <c r="Z46" s="157" t="s">
+        <v>590</v>
+      </c>
+      <c r="AA46" s="159">
+        <v>1.125E-2</v>
+      </c>
+      <c r="AB46" s="163">
+        <v>0.29489109000000002</v>
+      </c>
+      <c r="AC46" s="159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="2:29">
       <c r="B47" s="156" t="s">
         <v>172</v>
       </c>
@@ -9572,7 +11138,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="2:15">
+    <row r="48" spans="2:29">
       <c r="B48" s="157" t="s">
         <v>172</v>
       </c>
@@ -13969,7 +15535,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EF778A4-C78B-4C8A-8EFB-951DA82E413D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E5CDB70-31B1-4E5C-8DFE-C0ABFA789317}">
   <dimension ref="A1:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -14012,7 +15578,7 @@
         <v>153</v>
       </c>
       <c r="C10" s="155" t="s">
-        <v>518</v>
+        <v>591</v>
       </c>
       <c r="D10" s="155" t="s">
         <v>223</v>
@@ -14053,7 +15619,7 @@
     </row>
     <row r="11" spans="1:16">
       <c r="B11" s="156" t="s">
-        <v>519</v>
+        <v>592</v>
       </c>
       <c r="C11" s="156" t="s">
         <v>33</v>
@@ -14077,7 +15643,7 @@
         <v>172</v>
       </c>
       <c r="K11" s="156" t="s">
-        <v>519</v>
+        <v>592</v>
       </c>
       <c r="L11" s="156"/>
       <c r="M11" s="156" t="s">
@@ -14087,15 +15653,15 @@
         <v>21</v>
       </c>
       <c r="O11" s="156" t="s">
-        <v>541</v>
+        <v>614</v>
       </c>
       <c r="P11" s="156" t="s">
-        <v>542</v>
+        <v>615</v>
       </c>
     </row>
     <row r="12" spans="1:16">
       <c r="B12" s="157" t="s">
-        <v>519</v>
+        <v>592</v>
       </c>
       <c r="C12" s="157" t="s">
         <v>33</v>
@@ -14113,13 +15679,13 @@
         <v>0.60000000000000009</v>
       </c>
       <c r="H12" s="157" t="s">
-        <v>520</v>
+        <v>593</v>
       </c>
       <c r="J12" s="157" t="s">
         <v>172</v>
       </c>
       <c r="K12" s="157" t="s">
-        <v>524</v>
+        <v>597</v>
       </c>
       <c r="L12" s="157"/>
       <c r="M12" s="157" t="s">
@@ -14129,15 +15695,15 @@
         <v>21</v>
       </c>
       <c r="O12" s="157" t="s">
-        <v>541</v>
+        <v>614</v>
       </c>
       <c r="P12" s="157" t="s">
-        <v>542</v>
+        <v>615</v>
       </c>
     </row>
     <row r="13" spans="1:16">
       <c r="B13" s="156" t="s">
-        <v>519</v>
+        <v>592</v>
       </c>
       <c r="C13" s="156" t="s">
         <v>33</v>
@@ -14155,13 +15721,13 @@
         <v>5100</v>
       </c>
       <c r="H13" s="156" t="s">
-        <v>521</v>
+        <v>594</v>
       </c>
       <c r="J13" s="156" t="s">
         <v>172</v>
       </c>
       <c r="K13" s="156" t="s">
-        <v>525</v>
+        <v>598</v>
       </c>
       <c r="L13" s="156"/>
       <c r="M13" s="156" t="s">
@@ -14171,15 +15737,15 @@
         <v>21</v>
       </c>
       <c r="O13" s="156" t="s">
-        <v>541</v>
+        <v>614</v>
       </c>
       <c r="P13" s="156" t="s">
-        <v>542</v>
+        <v>615</v>
       </c>
     </row>
     <row r="14" spans="1:16">
       <c r="B14" s="157" t="s">
-        <v>519</v>
+        <v>592</v>
       </c>
       <c r="C14" s="157" t="s">
         <v>33</v>
@@ -14197,13 +15763,13 @@
         <v>175</v>
       </c>
       <c r="H14" s="157" t="s">
-        <v>522</v>
+        <v>595</v>
       </c>
       <c r="J14" s="157" t="s">
         <v>172</v>
       </c>
       <c r="K14" s="157" t="s">
-        <v>526</v>
+        <v>599</v>
       </c>
       <c r="L14" s="157"/>
       <c r="M14" s="157" t="s">
@@ -14213,15 +15779,15 @@
         <v>21</v>
       </c>
       <c r="O14" s="157" t="s">
-        <v>541</v>
+        <v>614</v>
       </c>
       <c r="P14" s="157" t="s">
-        <v>542</v>
+        <v>615</v>
       </c>
     </row>
     <row r="15" spans="1:16">
       <c r="B15" s="156" t="s">
-        <v>519</v>
+        <v>592</v>
       </c>
       <c r="C15" s="156" t="s">
         <v>33</v>
@@ -14239,13 +15805,13 @@
         <v>3</v>
       </c>
       <c r="H15" s="156" t="s">
-        <v>523</v>
+        <v>596</v>
       </c>
       <c r="J15" s="156" t="s">
         <v>172</v>
       </c>
       <c r="K15" s="156" t="s">
-        <v>527</v>
+        <v>600</v>
       </c>
       <c r="L15" s="156"/>
       <c r="M15" s="156" t="s">
@@ -14255,15 +15821,15 @@
         <v>21</v>
       </c>
       <c r="O15" s="156" t="s">
-        <v>541</v>
+        <v>614</v>
       </c>
       <c r="P15" s="156" t="s">
-        <v>542</v>
+        <v>615</v>
       </c>
     </row>
     <row r="16" spans="1:16">
       <c r="B16" s="157" t="s">
-        <v>524</v>
+        <v>597</v>
       </c>
       <c r="C16" s="157" t="s">
         <v>33</v>
@@ -14287,7 +15853,7 @@
         <v>172</v>
       </c>
       <c r="K16" s="157" t="s">
-        <v>528</v>
+        <v>601</v>
       </c>
       <c r="L16" s="157"/>
       <c r="M16" s="157" t="s">
@@ -14297,15 +15863,15 @@
         <v>21</v>
       </c>
       <c r="O16" s="157" t="s">
-        <v>541</v>
+        <v>614</v>
       </c>
       <c r="P16" s="157" t="s">
-        <v>542</v>
+        <v>615</v>
       </c>
     </row>
     <row r="17" spans="2:16">
       <c r="B17" s="156" t="s">
-        <v>524</v>
+        <v>597</v>
       </c>
       <c r="C17" s="156" t="s">
         <v>33</v>
@@ -14323,13 +15889,13 @@
         <v>0.60000000000000009</v>
       </c>
       <c r="H17" s="156" t="s">
-        <v>520</v>
+        <v>593</v>
       </c>
       <c r="J17" s="156" t="s">
         <v>172</v>
       </c>
       <c r="K17" s="156" t="s">
-        <v>529</v>
+        <v>602</v>
       </c>
       <c r="L17" s="156"/>
       <c r="M17" s="156" t="s">
@@ -14339,15 +15905,15 @@
         <v>21</v>
       </c>
       <c r="O17" s="156" t="s">
-        <v>541</v>
+        <v>614</v>
       </c>
       <c r="P17" s="156" t="s">
-        <v>542</v>
+        <v>615</v>
       </c>
     </row>
     <row r="18" spans="2:16">
       <c r="B18" s="157" t="s">
-        <v>524</v>
+        <v>597</v>
       </c>
       <c r="C18" s="157" t="s">
         <v>33</v>
@@ -14365,13 +15931,13 @@
         <v>2300</v>
       </c>
       <c r="H18" s="157" t="s">
-        <v>521</v>
+        <v>594</v>
       </c>
       <c r="J18" s="157" t="s">
         <v>172</v>
       </c>
       <c r="K18" s="157" t="s">
-        <v>530</v>
+        <v>603</v>
       </c>
       <c r="L18" s="157"/>
       <c r="M18" s="157" t="s">
@@ -14381,15 +15947,15 @@
         <v>21</v>
       </c>
       <c r="O18" s="157" t="s">
-        <v>541</v>
+        <v>614</v>
       </c>
       <c r="P18" s="157" t="s">
-        <v>542</v>
+        <v>615</v>
       </c>
     </row>
     <row r="19" spans="2:16">
       <c r="B19" s="156" t="s">
-        <v>524</v>
+        <v>597</v>
       </c>
       <c r="C19" s="156" t="s">
         <v>33</v>
@@ -14407,13 +15973,13 @@
         <v>80</v>
       </c>
       <c r="H19" s="156" t="s">
-        <v>522</v>
+        <v>595</v>
       </c>
       <c r="J19" s="156" t="s">
         <v>172</v>
       </c>
       <c r="K19" s="156" t="s">
-        <v>531</v>
+        <v>604</v>
       </c>
       <c r="L19" s="156"/>
       <c r="M19" s="156" t="s">
@@ -14423,15 +15989,15 @@
         <v>21</v>
       </c>
       <c r="O19" s="156" t="s">
-        <v>541</v>
+        <v>614</v>
       </c>
       <c r="P19" s="156" t="s">
-        <v>542</v>
+        <v>615</v>
       </c>
     </row>
     <row r="20" spans="2:16">
       <c r="B20" s="157" t="s">
-        <v>524</v>
+        <v>597</v>
       </c>
       <c r="C20" s="157" t="s">
         <v>33</v>
@@ -14449,13 +16015,13 @@
         <v>3</v>
       </c>
       <c r="H20" s="157" t="s">
-        <v>523</v>
+        <v>596</v>
       </c>
       <c r="J20" s="157" t="s">
         <v>172</v>
       </c>
       <c r="K20" s="157" t="s">
-        <v>532</v>
+        <v>605</v>
       </c>
       <c r="L20" s="157"/>
       <c r="M20" s="157" t="s">
@@ -14465,15 +16031,15 @@
         <v>21</v>
       </c>
       <c r="O20" s="157" t="s">
-        <v>541</v>
+        <v>614</v>
       </c>
       <c r="P20" s="157" t="s">
-        <v>542</v>
+        <v>615</v>
       </c>
     </row>
     <row r="21" spans="2:16">
       <c r="B21" s="156" t="s">
-        <v>525</v>
+        <v>598</v>
       </c>
       <c r="C21" s="156" t="s">
         <v>35</v>
@@ -14497,7 +16063,7 @@
         <v>172</v>
       </c>
       <c r="K21" s="156" t="s">
-        <v>533</v>
+        <v>606</v>
       </c>
       <c r="L21" s="156"/>
       <c r="M21" s="156" t="s">
@@ -14507,15 +16073,15 @@
         <v>21</v>
       </c>
       <c r="O21" s="156" t="s">
-        <v>541</v>
+        <v>614</v>
       </c>
       <c r="P21" s="156" t="s">
-        <v>542</v>
+        <v>615</v>
       </c>
     </row>
     <row r="22" spans="2:16">
       <c r="B22" s="157" t="s">
-        <v>525</v>
+        <v>598</v>
       </c>
       <c r="C22" s="157" t="s">
         <v>35</v>
@@ -14533,13 +16099,13 @@
         <v>1000</v>
       </c>
       <c r="H22" s="157" t="s">
-        <v>521</v>
+        <v>594</v>
       </c>
       <c r="J22" s="157" t="s">
         <v>172</v>
       </c>
       <c r="K22" s="157" t="s">
-        <v>534</v>
+        <v>607</v>
       </c>
       <c r="L22" s="157"/>
       <c r="M22" s="157" t="s">
@@ -14549,15 +16115,15 @@
         <v>21</v>
       </c>
       <c r="O22" s="157" t="s">
-        <v>541</v>
+        <v>614</v>
       </c>
       <c r="P22" s="157" t="s">
-        <v>542</v>
+        <v>615</v>
       </c>
     </row>
     <row r="23" spans="2:16">
       <c r="B23" s="156" t="s">
-        <v>525</v>
+        <v>598</v>
       </c>
       <c r="C23" s="156" t="s">
         <v>35</v>
@@ -14575,13 +16141,13 @@
         <v>25</v>
       </c>
       <c r="H23" s="156" t="s">
-        <v>522</v>
+        <v>595</v>
       </c>
       <c r="J23" s="156" t="s">
         <v>172</v>
       </c>
       <c r="K23" s="156" t="s">
-        <v>535</v>
+        <v>608</v>
       </c>
       <c r="L23" s="156"/>
       <c r="M23" s="156" t="s">
@@ -14591,15 +16157,15 @@
         <v>21</v>
       </c>
       <c r="O23" s="156" t="s">
-        <v>541</v>
+        <v>614</v>
       </c>
       <c r="P23" s="156" t="s">
-        <v>542</v>
+        <v>615</v>
       </c>
     </row>
     <row r="24" spans="2:16">
       <c r="B24" s="157" t="s">
-        <v>526</v>
+        <v>599</v>
       </c>
       <c r="C24" s="157" t="s">
         <v>35</v>
@@ -14623,7 +16189,7 @@
         <v>172</v>
       </c>
       <c r="K24" s="157" t="s">
-        <v>536</v>
+        <v>609</v>
       </c>
       <c r="L24" s="157"/>
       <c r="M24" s="157" t="s">
@@ -14633,15 +16199,15 @@
         <v>21</v>
       </c>
       <c r="O24" s="157" t="s">
-        <v>541</v>
+        <v>614</v>
       </c>
       <c r="P24" s="157" t="s">
-        <v>542</v>
+        <v>615</v>
       </c>
     </row>
     <row r="25" spans="2:16">
       <c r="B25" s="156" t="s">
-        <v>526</v>
+        <v>599</v>
       </c>
       <c r="C25" s="156" t="s">
         <v>35</v>
@@ -14659,13 +16225,13 @@
         <v>2400</v>
       </c>
       <c r="H25" s="156" t="s">
-        <v>521</v>
+        <v>594</v>
       </c>
       <c r="J25" s="156" t="s">
         <v>172</v>
       </c>
       <c r="K25" s="156" t="s">
-        <v>537</v>
+        <v>610</v>
       </c>
       <c r="L25" s="156"/>
       <c r="M25" s="156" t="s">
@@ -14675,15 +16241,15 @@
         <v>21</v>
       </c>
       <c r="O25" s="156" t="s">
-        <v>541</v>
+        <v>614</v>
       </c>
       <c r="P25" s="156" t="s">
-        <v>542</v>
+        <v>615</v>
       </c>
     </row>
     <row r="26" spans="2:16">
       <c r="B26" s="157" t="s">
-        <v>526</v>
+        <v>599</v>
       </c>
       <c r="C26" s="157" t="s">
         <v>35</v>
@@ -14701,13 +16267,13 @@
         <v>60</v>
       </c>
       <c r="H26" s="157" t="s">
-        <v>522</v>
+        <v>595</v>
       </c>
       <c r="J26" s="157" t="s">
         <v>172</v>
       </c>
       <c r="K26" s="157" t="s">
-        <v>538</v>
+        <v>611</v>
       </c>
       <c r="L26" s="157"/>
       <c r="M26" s="157" t="s">
@@ -14717,15 +16283,15 @@
         <v>21</v>
       </c>
       <c r="O26" s="157" t="s">
-        <v>541</v>
+        <v>614</v>
       </c>
       <c r="P26" s="157" t="s">
-        <v>542</v>
+        <v>615</v>
       </c>
     </row>
     <row r="27" spans="2:16">
       <c r="B27" s="156" t="s">
-        <v>527</v>
+        <v>600</v>
       </c>
       <c r="C27" s="156" t="s">
         <v>34</v>
@@ -14749,7 +16315,7 @@
         <v>172</v>
       </c>
       <c r="K27" s="156" t="s">
-        <v>540</v>
+        <v>613</v>
       </c>
       <c r="L27" s="156"/>
       <c r="M27" s="156" t="s">
@@ -14759,15 +16325,15 @@
         <v>21</v>
       </c>
       <c r="O27" s="156" t="s">
-        <v>541</v>
+        <v>614</v>
       </c>
       <c r="P27" s="156" t="s">
-        <v>542</v>
+        <v>615</v>
       </c>
     </row>
     <row r="28" spans="2:16">
       <c r="B28" s="157" t="s">
-        <v>527</v>
+        <v>600</v>
       </c>
       <c r="C28" s="157" t="s">
         <v>34</v>
@@ -14785,12 +16351,12 @@
         <v>4350</v>
       </c>
       <c r="H28" s="157" t="s">
-        <v>521</v>
+        <v>594</v>
       </c>
     </row>
     <row r="29" spans="2:16">
       <c r="B29" s="156" t="s">
-        <v>527</v>
+        <v>600</v>
       </c>
       <c r="C29" s="156" t="s">
         <v>34</v>
@@ -14808,12 +16374,12 @@
         <v>130</v>
       </c>
       <c r="H29" s="156" t="s">
-        <v>522</v>
+        <v>595</v>
       </c>
     </row>
     <row r="30" spans="2:16">
       <c r="B30" s="157" t="s">
-        <v>528</v>
+        <v>601</v>
       </c>
       <c r="C30" s="157" t="s">
         <v>35</v>
@@ -14836,7 +16402,7 @@
     </row>
     <row r="31" spans="2:16">
       <c r="B31" s="156" t="s">
-        <v>528</v>
+        <v>601</v>
       </c>
       <c r="C31" s="156" t="s">
         <v>35</v>
@@ -14854,12 +16420,12 @@
         <v>500</v>
       </c>
       <c r="H31" s="156" t="s">
-        <v>521</v>
+        <v>594</v>
       </c>
     </row>
     <row r="32" spans="2:16">
       <c r="B32" s="157" t="s">
-        <v>528</v>
+        <v>601</v>
       </c>
       <c r="C32" s="157" t="s">
         <v>35</v>
@@ -14877,12 +16443,12 @@
         <v>20</v>
       </c>
       <c r="H32" s="157" t="s">
-        <v>522</v>
+        <v>595</v>
       </c>
     </row>
     <row r="33" spans="2:8">
       <c r="B33" s="156" t="s">
-        <v>529</v>
+        <v>602</v>
       </c>
       <c r="C33" s="156" t="s">
         <v>29</v>
@@ -14905,7 +16471,7 @@
     </row>
     <row r="34" spans="2:8">
       <c r="B34" s="157" t="s">
-        <v>529</v>
+        <v>602</v>
       </c>
       <c r="C34" s="157" t="s">
         <v>29</v>
@@ -14923,12 +16489,12 @@
         <v>0.35000000000000003</v>
       </c>
       <c r="H34" s="157" t="s">
-        <v>520</v>
+        <v>593</v>
       </c>
     </row>
     <row r="35" spans="2:8">
       <c r="B35" s="156" t="s">
-        <v>529</v>
+        <v>602</v>
       </c>
       <c r="C35" s="156" t="s">
         <v>29</v>
@@ -14946,12 +16512,12 @@
         <v>2650</v>
       </c>
       <c r="H35" s="156" t="s">
-        <v>521</v>
+        <v>594</v>
       </c>
     </row>
     <row r="36" spans="2:8">
       <c r="B36" s="157" t="s">
-        <v>529</v>
+        <v>602</v>
       </c>
       <c r="C36" s="157" t="s">
         <v>29</v>
@@ -14969,12 +16535,12 @@
         <v>65</v>
       </c>
       <c r="H36" s="157" t="s">
-        <v>522</v>
+        <v>595</v>
       </c>
     </row>
     <row r="37" spans="2:8">
       <c r="B37" s="156" t="s">
-        <v>529</v>
+        <v>602</v>
       </c>
       <c r="C37" s="156" t="s">
         <v>29</v>
@@ -14992,12 +16558,12 @@
         <v>4</v>
       </c>
       <c r="H37" s="156" t="s">
-        <v>523</v>
+        <v>596</v>
       </c>
     </row>
     <row r="38" spans="2:8">
       <c r="B38" s="157" t="s">
-        <v>530</v>
+        <v>603</v>
       </c>
       <c r="C38" s="157" t="s">
         <v>35</v>
@@ -15020,7 +16586,7 @@
     </row>
     <row r="39" spans="2:8">
       <c r="B39" s="156" t="s">
-        <v>530</v>
+        <v>603</v>
       </c>
       <c r="C39" s="156" t="s">
         <v>35</v>
@@ -15038,12 +16604,12 @@
         <v>2300</v>
       </c>
       <c r="H39" s="156" t="s">
-        <v>521</v>
+        <v>594</v>
       </c>
     </row>
     <row r="40" spans="2:8">
       <c r="B40" s="157" t="s">
-        <v>530</v>
+        <v>603</v>
       </c>
       <c r="C40" s="157" t="s">
         <v>35</v>
@@ -15061,12 +16627,12 @@
         <v>80</v>
       </c>
       <c r="H40" s="157" t="s">
-        <v>522</v>
+        <v>595</v>
       </c>
     </row>
     <row r="41" spans="2:8">
       <c r="B41" s="156" t="s">
-        <v>531</v>
+        <v>604</v>
       </c>
       <c r="C41" s="156" t="s">
         <v>34</v>
@@ -15089,7 +16655,7 @@
     </row>
     <row r="42" spans="2:8">
       <c r="B42" s="157" t="s">
-        <v>531</v>
+        <v>604</v>
       </c>
       <c r="C42" s="157" t="s">
         <v>34</v>
@@ -15107,12 +16673,12 @@
         <v>5100</v>
       </c>
       <c r="H42" s="157" t="s">
-        <v>521</v>
+        <v>594</v>
       </c>
     </row>
     <row r="43" spans="2:8">
       <c r="B43" s="156" t="s">
-        <v>531</v>
+        <v>604</v>
       </c>
       <c r="C43" s="156" t="s">
         <v>34</v>
@@ -15130,12 +16696,12 @@
         <v>180</v>
       </c>
       <c r="H43" s="156" t="s">
-        <v>522</v>
+        <v>595</v>
       </c>
     </row>
     <row r="44" spans="2:8">
       <c r="B44" s="157" t="s">
-        <v>532</v>
+        <v>605</v>
       </c>
       <c r="C44" s="157" t="s">
         <v>38</v>
@@ -15158,7 +16724,7 @@
     </row>
     <row r="45" spans="2:8">
       <c r="B45" s="156" t="s">
-        <v>532</v>
+        <v>605</v>
       </c>
       <c r="C45" s="156" t="s">
         <v>38</v>
@@ -15176,12 +16742,12 @@
         <v>4500</v>
       </c>
       <c r="H45" s="156" t="s">
-        <v>521</v>
+        <v>594</v>
       </c>
     </row>
     <row r="46" spans="2:8">
       <c r="B46" s="157" t="s">
-        <v>532</v>
+        <v>605</v>
       </c>
       <c r="C46" s="157" t="s">
         <v>38</v>
@@ -15199,12 +16765,12 @@
         <v>160</v>
       </c>
       <c r="H46" s="157" t="s">
-        <v>522</v>
+        <v>595</v>
       </c>
     </row>
     <row r="47" spans="2:8">
       <c r="B47" s="156" t="s">
-        <v>533</v>
+        <v>606</v>
       </c>
       <c r="C47" s="156" t="s">
         <v>34</v>
@@ -15227,7 +16793,7 @@
     </row>
     <row r="48" spans="2:8">
       <c r="B48" s="157" t="s">
-        <v>533</v>
+        <v>606</v>
       </c>
       <c r="C48" s="157" t="s">
         <v>34</v>
@@ -15245,12 +16811,12 @@
         <v>5100</v>
       </c>
       <c r="H48" s="157" t="s">
-        <v>521</v>
+        <v>594</v>
       </c>
     </row>
     <row r="49" spans="2:8">
       <c r="B49" s="156" t="s">
-        <v>533</v>
+        <v>606</v>
       </c>
       <c r="C49" s="156" t="s">
         <v>34</v>
@@ -15268,12 +16834,12 @@
         <v>155</v>
       </c>
       <c r="H49" s="156" t="s">
-        <v>522</v>
+        <v>595</v>
       </c>
     </row>
     <row r="50" spans="2:8">
       <c r="B50" s="157" t="s">
-        <v>534</v>
+        <v>607</v>
       </c>
       <c r="C50" s="157" t="s">
         <v>27</v>
@@ -15296,7 +16862,7 @@
     </row>
     <row r="51" spans="2:8">
       <c r="B51" s="156" t="s">
-        <v>534</v>
+        <v>607</v>
       </c>
       <c r="C51" s="156" t="s">
         <v>27</v>
@@ -15314,12 +16880,12 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="H51" s="156" t="s">
-        <v>520</v>
+        <v>593</v>
       </c>
     </row>
     <row r="52" spans="2:8">
       <c r="B52" s="157" t="s">
-        <v>534</v>
+        <v>607</v>
       </c>
       <c r="C52" s="157" t="s">
         <v>27</v>
@@ -15337,12 +16903,12 @@
         <v>340</v>
       </c>
       <c r="H52" s="157" t="s">
-        <v>521</v>
+        <v>594</v>
       </c>
     </row>
     <row r="53" spans="2:8">
       <c r="B53" s="156" t="s">
-        <v>534</v>
+        <v>607</v>
       </c>
       <c r="C53" s="156" t="s">
         <v>27</v>
@@ -15360,12 +16926,12 @@
         <v>10</v>
       </c>
       <c r="H53" s="156" t="s">
-        <v>522</v>
+        <v>595</v>
       </c>
     </row>
     <row r="54" spans="2:8">
       <c r="B54" s="157" t="s">
-        <v>534</v>
+        <v>607</v>
       </c>
       <c r="C54" s="157" t="s">
         <v>27</v>
@@ -15383,12 +16949,12 @@
         <v>1.5</v>
       </c>
       <c r="H54" s="157" t="s">
-        <v>523</v>
+        <v>596</v>
       </c>
     </row>
     <row r="55" spans="2:8">
       <c r="B55" s="156" t="s">
-        <v>535</v>
+        <v>608</v>
       </c>
       <c r="C55" s="156" t="s">
         <v>34</v>
@@ -15411,7 +16977,7 @@
     </row>
     <row r="56" spans="2:8">
       <c r="B56" s="157" t="s">
-        <v>535</v>
+        <v>608</v>
       </c>
       <c r="C56" s="157" t="s">
         <v>34</v>
@@ -15429,12 +16995,12 @@
         <v>1700</v>
       </c>
       <c r="H56" s="157" t="s">
-        <v>521</v>
+        <v>594</v>
       </c>
     </row>
     <row r="57" spans="2:8">
       <c r="B57" s="156" t="s">
-        <v>535</v>
+        <v>608</v>
       </c>
       <c r="C57" s="156" t="s">
         <v>34</v>
@@ -15452,12 +17018,12 @@
         <v>45</v>
       </c>
       <c r="H57" s="156" t="s">
-        <v>522</v>
+        <v>595</v>
       </c>
     </row>
     <row r="58" spans="2:8">
       <c r="B58" s="157" t="s">
-        <v>536</v>
+        <v>609</v>
       </c>
       <c r="C58" s="157" t="s">
         <v>34</v>
@@ -15480,7 +17046,7 @@
     </row>
     <row r="59" spans="2:8">
       <c r="B59" s="156" t="s">
-        <v>536</v>
+        <v>609</v>
       </c>
       <c r="C59" s="156" t="s">
         <v>34</v>
@@ -15498,12 +17064,12 @@
         <v>2000</v>
       </c>
       <c r="H59" s="156" t="s">
-        <v>521</v>
+        <v>594</v>
       </c>
     </row>
     <row r="60" spans="2:8">
       <c r="B60" s="157" t="s">
-        <v>536</v>
+        <v>609</v>
       </c>
       <c r="C60" s="157" t="s">
         <v>34</v>
@@ -15521,12 +17087,12 @@
         <v>60</v>
       </c>
       <c r="H60" s="157" t="s">
-        <v>522</v>
+        <v>595</v>
       </c>
     </row>
     <row r="61" spans="2:8">
       <c r="B61" s="156" t="s">
-        <v>537</v>
+        <v>610</v>
       </c>
       <c r="C61" s="156" t="s">
         <v>34</v>
@@ -15549,7 +17115,7 @@
     </row>
     <row r="62" spans="2:8">
       <c r="B62" s="157" t="s">
-        <v>537</v>
+        <v>610</v>
       </c>
       <c r="C62" s="157" t="s">
         <v>34</v>
@@ -15567,12 +17133,12 @@
         <v>2200</v>
       </c>
       <c r="H62" s="157" t="s">
-        <v>521</v>
+        <v>594</v>
       </c>
     </row>
     <row r="63" spans="2:8">
       <c r="B63" s="156" t="s">
-        <v>537</v>
+        <v>610</v>
       </c>
       <c r="C63" s="156" t="s">
         <v>34</v>
@@ -15590,15 +17156,15 @@
         <v>65</v>
       </c>
       <c r="H63" s="156" t="s">
-        <v>522</v>
+        <v>595</v>
       </c>
     </row>
     <row r="64" spans="2:8">
       <c r="B64" s="157" t="s">
-        <v>538</v>
+        <v>611</v>
       </c>
       <c r="C64" s="157" t="s">
-        <v>539</v>
+        <v>612</v>
       </c>
       <c r="D64" s="157" t="s">
         <v>19</v>
@@ -15618,10 +17184,10 @@
     </row>
     <row r="65" spans="2:8">
       <c r="B65" s="156" t="s">
-        <v>538</v>
+        <v>611</v>
       </c>
       <c r="C65" s="156" t="s">
-        <v>539</v>
+        <v>612</v>
       </c>
       <c r="D65" s="156" t="s">
         <v>19</v>
@@ -15636,15 +17202,15 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="H65" s="156" t="s">
-        <v>520</v>
+        <v>593</v>
       </c>
     </row>
     <row r="66" spans="2:8">
       <c r="B66" s="157" t="s">
-        <v>538</v>
+        <v>611</v>
       </c>
       <c r="C66" s="157" t="s">
-        <v>539</v>
+        <v>612</v>
       </c>
       <c r="D66" s="157" t="s">
         <v>19</v>
@@ -15659,15 +17225,15 @@
         <v>1660</v>
       </c>
       <c r="H66" s="157" t="s">
-        <v>521</v>
+        <v>594</v>
       </c>
     </row>
     <row r="67" spans="2:8">
       <c r="B67" s="156" t="s">
-        <v>538</v>
+        <v>611</v>
       </c>
       <c r="C67" s="156" t="s">
-        <v>539</v>
+        <v>612</v>
       </c>
       <c r="D67" s="156" t="s">
         <v>19</v>
@@ -15682,15 +17248,15 @@
         <v>40</v>
       </c>
       <c r="H67" s="156" t="s">
-        <v>522</v>
+        <v>595</v>
       </c>
     </row>
     <row r="68" spans="2:8">
       <c r="B68" s="157" t="s">
-        <v>538</v>
+        <v>611</v>
       </c>
       <c r="C68" s="157" t="s">
-        <v>539</v>
+        <v>612</v>
       </c>
       <c r="D68" s="157" t="s">
         <v>19</v>
@@ -15705,15 +17271,15 @@
         <v>3</v>
       </c>
       <c r="H68" s="157" t="s">
-        <v>523</v>
+        <v>596</v>
       </c>
     </row>
     <row r="69" spans="2:8">
       <c r="B69" s="156" t="s">
-        <v>540</v>
+        <v>613</v>
       </c>
       <c r="C69" s="156" t="s">
-        <v>539</v>
+        <v>612</v>
       </c>
       <c r="D69" s="156" t="s">
         <v>19</v>
@@ -15733,10 +17299,10 @@
     </row>
     <row r="70" spans="2:8">
       <c r="B70" s="157" t="s">
-        <v>540</v>
+        <v>613</v>
       </c>
       <c r="C70" s="157" t="s">
-        <v>539</v>
+        <v>612</v>
       </c>
       <c r="D70" s="157" t="s">
         <v>19</v>
@@ -15751,15 +17317,15 @@
         <v>0.3</v>
       </c>
       <c r="H70" s="157" t="s">
-        <v>520</v>
+        <v>593</v>
       </c>
     </row>
     <row r="71" spans="2:8">
       <c r="B71" s="156" t="s">
-        <v>540</v>
+        <v>613</v>
       </c>
       <c r="C71" s="156" t="s">
-        <v>539</v>
+        <v>612</v>
       </c>
       <c r="D71" s="156" t="s">
         <v>19</v>
@@ -15774,15 +17340,15 @@
         <v>1490</v>
       </c>
       <c r="H71" s="156" t="s">
-        <v>521</v>
+        <v>594</v>
       </c>
     </row>
     <row r="72" spans="2:8">
       <c r="B72" s="157" t="s">
-        <v>540</v>
+        <v>613</v>
       </c>
       <c r="C72" s="157" t="s">
-        <v>539</v>
+        <v>612</v>
       </c>
       <c r="D72" s="157" t="s">
         <v>19</v>
@@ -15797,15 +17363,15 @@
         <v>38</v>
       </c>
       <c r="H72" s="157" t="s">
-        <v>522</v>
+        <v>595</v>
       </c>
     </row>
     <row r="73" spans="2:8">
       <c r="B73" s="156" t="s">
-        <v>540</v>
+        <v>613</v>
       </c>
       <c r="C73" s="156" t="s">
-        <v>539</v>
+        <v>612</v>
       </c>
       <c r="D73" s="156" t="s">
         <v>19</v>
@@ -15820,7 +17386,7 @@
         <v>1.5</v>
       </c>
       <c r="H73" s="156" t="s">
-        <v>523</v>
+        <v>596</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated DEU model - 2025-08-31 19:51
</commit_message>
<xml_diff>
--- a/VerveStacks_DEU/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_DEU/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_DEU\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7FB87C35-88B3-4BAD-84FA-21BE7444021E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{078C34FB-F2FE-4E4A-929A-1E1C54280D12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3019,7 +3019,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{580E2BD9-B885-6EE0-BDCD-45052E27766A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{876FE61A-E049-3447-AE4F-99DB0B717FC5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3074,7 +3074,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43FABB0C-987F-6E33-35AA-8BF5267D8504}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CE03331-9FF1-52FA-C3AC-BA4B76E25A91}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3129,7 +3129,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1F4CA59-85F2-E984-96A9-0E244ABE5476}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7883C82D-7037-3BCB-6EE7-2EF78B36B7BC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3184,7 +3184,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46FD4F18-AF89-1422-04AA-C4CC8C12F9FF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EB0F6A2-A781-FDC6-C7EA-5FE46600FFC6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7114,7 +7114,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD8905F6-3653-4930-97B5-EB6447F2C35D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9822D14A-7F03-4965-9CFF-95B00AF7DC71}">
   <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8191,7 +8191,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899E3FFA-71C8-40E0-BF81-6954D2208FCA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63A528B8-7D44-4AE0-909B-89EB5192152F}">
   <dimension ref="A1:AC154"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15535,7 +15535,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E5CDB70-31B1-4E5C-8DFE-C0ABFA789317}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2AB0281-B3C3-4BFB-B69D-B8AA5173E726}">
   <dimension ref="A1:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated DEU model - 2025-08-31 20:37
</commit_message>
<xml_diff>
--- a/VerveStacks_DEU/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_DEU/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_DEU\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{078C34FB-F2FE-4E4A-929A-1E1C54280D12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{702ECD12-6800-40E6-AF57-F7BE9BCB27A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3019,7 +3019,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{876FE61A-E049-3447-AE4F-99DB0B717FC5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{919AC051-24CD-2A8B-E3D3-9B0974C0FDB9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3074,7 +3074,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CE03331-9FF1-52FA-C3AC-BA4B76E25A91}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C31DA64-95A9-C93C-2B01-F31D85A664F4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3129,7 +3129,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7883C82D-7037-3BCB-6EE7-2EF78B36B7BC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5227BB17-DD67-695D-F14F-12DEF6CCF753}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3184,7 +3184,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EB0F6A2-A781-FDC6-C7EA-5FE46600FFC6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7F0F294-D41C-858C-484B-2EE2EF205EE5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7114,7 +7114,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9822D14A-7F03-4965-9CFF-95B00AF7DC71}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC60CD7-A2B4-4EAD-AF36-A03EB802FB98}">
   <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8191,7 +8191,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63A528B8-7D44-4AE0-909B-89EB5192152F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D58F27DC-F219-4AD3-98FB-808DF58CD13B}">
   <dimension ref="A1:AC154"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15535,7 +15535,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2AB0281-B3C3-4BFB-B69D-B8AA5173E726}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3DA05FA-545A-47C5-AE6D-3C5940237EC4}">
   <dimension ref="A1:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated DEU model - 2025-09-01 00:55
</commit_message>
<xml_diff>
--- a/VerveStacks_DEU/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_DEU/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_DEU\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3DB88CD1-9C0C-48F8-B97F-8C684E671AD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C6EE88E-EAE6-462D-AC7C-D2F03B444FBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3022,7 +3022,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B160C630-9A11-6493-504A-DD20BC69CAEB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FFEFAB3-FCD9-A5E3-4D5E-22781F2C2A21}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3077,7 +3077,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{773D0F34-7F57-0EEE-126E-CE2B3B589747}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9BFF308-30E0-AC3D-AB6E-7B3FC242B82A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3132,7 +3132,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{548A6A56-BD7A-7E98-BDA1-239E9C69A5F9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43A31C04-5ABB-3C44-D8C3-7F613FF70F2A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3187,7 +3187,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48718462-DDB7-DC07-52CC-5DADAA046D4A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A16696F2-499D-0343-788F-39E206FADB7E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7117,7 +7117,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98E58F44-C1B3-4FCD-834D-8D87D3E45505}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F19FDBC-2233-4882-9638-718A84BE06BA}">
   <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8117,7 +8117,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A83B6D7A-0698-40FF-A6BC-BB7D45B66468}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B780D27-D910-41E2-A4DD-93E1A0D0A275}">
   <dimension ref="A1:AB154"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15060,7 +15060,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD309F23-38AC-4F26-A3EC-8DD623C72707}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{918D8F42-BD08-463B-B813-4B8A9BDB9E5F}">
   <dimension ref="A1:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>